<commit_message>
[FIX] template line unit base with org
</commit_message>
<xml_diff>
--- a/pabi_budget_plan/xlsx_template/budget_control_unit_base.xlsx
+++ b/pabi_budget_plan/xlsx_template/budget_control_unit_base.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t xml:space="preserve">Budget Control</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t xml:space="preserve">Sep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Org</t>
   </si>
 </sst>
 </file>
@@ -133,7 +136,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.00_);\(#,##0.00\)"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -204,13 +207,6 @@
       <name val="Monospaced"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Monospaced"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="4">
@@ -267,7 +263,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -348,10 +344,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -366,12 +358,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -441,13 +433,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W10"/>
+  <dimension ref="A1:X10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="19.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="21.06"/>
@@ -460,8 +452,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="25.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="25.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="13.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="14" style="3" width="19.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="24" style="0" width="19.91"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="23" min="14" style="3" width="19.91"/>
   </cols>
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -692,7 +683,7 @@
       <c r="V9" s="18"/>
       <c r="W9" s="18"/>
     </row>
-    <row r="10" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="19" t="s">
         <v>12</v>
       </c>
@@ -711,7 +702,7 @@
       <c r="F10" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="20" t="s">
+      <c r="G10" s="19" t="s">
         <v>18</v>
       </c>
       <c r="H10" s="19" t="s">
@@ -720,47 +711,50 @@
       <c r="I10" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="21" t="s">
+      <c r="J10" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="K10" s="21" t="s">
+      <c r="K10" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="L10" s="22" t="s">
+      <c r="L10" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="M10" s="23" t="s">
+      <c r="M10" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="N10" s="23" t="s">
+      <c r="N10" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="O10" s="23" t="s">
+      <c r="O10" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="P10" s="23" t="s">
+      <c r="P10" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="Q10" s="23" t="s">
+      <c r="Q10" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="R10" s="23" t="s">
+      <c r="R10" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="S10" s="23" t="s">
+      <c r="S10" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="T10" s="23" t="s">
+      <c r="T10" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="U10" s="23" t="s">
+      <c r="U10" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="V10" s="23" t="s">
+      <c r="V10" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="W10" s="23" t="s">
+      <c r="W10" s="22" t="s">
         <v>33</v>
+      </c>
+      <c r="X10" s="22" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>